<commit_message>
modified MCA & added analysis on CAD exp
</commit_message>
<xml_diff>
--- a/data/SURVEY RESULTS_2024.xlsx
+++ b/data/SURVEY RESULTS_2024.xlsx
@@ -787,11 +787,11 @@
     <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="61.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="61.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="45.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="62.57642857142857" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
@@ -2177,7 +2177,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="M38" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1" t="s">
         <v>57</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="M40" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="M41" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="M42" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>120</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="M45" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
         <v>13</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
         <v>13</v>
       </c>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="M47" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>